<commit_message>
Started work on #12 and #14
</commit_message>
<xml_diff>
--- a/Color_Scale.xlsx
+++ b/Color_Scale.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\espeh\github\clocky\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05CC6649-2BD6-4A60-96BB-2586AB1CE2D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BEDF049-46E4-4008-B22A-0817F74FA744}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21360" windowHeight="10500" xr2:uid="{5FCEDDE9-D0E5-4628-A5ED-12D85F3EE388}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23505" windowHeight="21000" xr2:uid="{5FCEDDE9-D0E5-4628-A5ED-12D85F3EE388}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="25">
   <si>
     <t>target_hours</t>
   </si>
@@ -60,6 +60,57 @@
   </si>
   <si>
     <t>default →</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>light black</t>
+  </si>
+  <si>
+    <t>white</t>
+  </si>
+  <si>
+    <t>light white</t>
+  </si>
+  <si>
+    <t>magenta</t>
+  </si>
+  <si>
+    <t>blue</t>
+  </si>
+  <si>
+    <t>light blue</t>
+  </si>
+  <si>
+    <t>light cyan</t>
+  </si>
+  <si>
+    <t>cyan</t>
+  </si>
+  <si>
+    <t>green</t>
+  </si>
+  <si>
+    <t>light green</t>
+  </si>
+  <si>
+    <t>light yellow</t>
+  </si>
+  <si>
+    <t>yellow</t>
+  </si>
+  <si>
+    <t>red</t>
+  </si>
+  <si>
+    <t>light red</t>
+  </si>
+  <si>
+    <t>light magenta</t>
+  </si>
+  <si>
+    <t>I</t>
   </si>
 </sst>
 </file>
@@ -67,9 +118,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.000000"/>
+    <numFmt numFmtId="164" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -90,6 +141,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-4.9989318521683403E-2"/>
+      <name val="Cascadia Mono"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="19">
@@ -233,10 +290,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment textRotation="255"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment textRotation="255"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -263,12 +317,43 @@
     <xf numFmtId="0" fontId="2" fillId="16" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="17" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="18" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Input" xfId="1" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -619,10 +704,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7803A6AB-4C79-437F-A45F-ED6E12B6E924}">
-  <dimension ref="A3:AZ13"/>
+  <dimension ref="A3:AZ34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="Z16" sqref="Z16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M41" sqref="M41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -643,10 +728,10 @@
       </c>
     </row>
     <row r="9" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C9" s="2">
@@ -801,86 +886,86 @@
       </c>
     </row>
     <row r="10" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6">
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5">
         <v>1</v>
       </c>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6">
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5">
         <v>2</v>
       </c>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="6">
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5">
         <v>3</v>
       </c>
-      <c r="O10" s="6"/>
-      <c r="P10" s="6"/>
-      <c r="Q10" s="6"/>
-      <c r="R10" s="6">
+      <c r="O10" s="5"/>
+      <c r="P10" s="5"/>
+      <c r="Q10" s="5"/>
+      <c r="R10" s="5">
         <v>4</v>
       </c>
-      <c r="S10" s="6"/>
-      <c r="T10" s="6"/>
-      <c r="U10" s="6"/>
-      <c r="V10" s="6">
+      <c r="S10" s="5"/>
+      <c r="T10" s="5"/>
+      <c r="U10" s="5"/>
+      <c r="V10" s="5">
         <v>5</v>
       </c>
-      <c r="W10" s="6"/>
-      <c r="X10" s="6"/>
-      <c r="Y10" s="6"/>
-      <c r="Z10" s="6">
-        <v>6</v>
-      </c>
-      <c r="AA10" s="6"/>
-      <c r="AB10" s="6"/>
-      <c r="AC10" s="6"/>
-      <c r="AD10" s="6">
+      <c r="W10" s="5"/>
+      <c r="X10" s="5"/>
+      <c r="Y10" s="5"/>
+      <c r="Z10" s="5">
+        <v>6</v>
+      </c>
+      <c r="AA10" s="5"/>
+      <c r="AB10" s="5"/>
+      <c r="AC10" s="5"/>
+      <c r="AD10" s="5">
         <v>7</v>
       </c>
-      <c r="AE10" s="6"/>
-      <c r="AF10" s="6"/>
-      <c r="AG10" s="6"/>
-      <c r="AH10" s="6">
-        <v>8</v>
-      </c>
-      <c r="AI10" s="6"/>
-      <c r="AJ10" s="6"/>
-      <c r="AK10" s="6"/>
-      <c r="AL10" s="6">
+      <c r="AE10" s="5"/>
+      <c r="AF10" s="5"/>
+      <c r="AG10" s="5"/>
+      <c r="AH10" s="5">
+        <v>8</v>
+      </c>
+      <c r="AI10" s="5"/>
+      <c r="AJ10" s="5"/>
+      <c r="AK10" s="5"/>
+      <c r="AL10" s="5">
         <v>9</v>
       </c>
-      <c r="AM10" s="6"/>
-      <c r="AN10" s="6"/>
-      <c r="AO10" s="6"/>
-      <c r="AP10" s="6">
+      <c r="AM10" s="5"/>
+      <c r="AN10" s="5"/>
+      <c r="AO10" s="5"/>
+      <c r="AP10" s="5">
         <v>10</v>
       </c>
-      <c r="AQ10" s="6"/>
-      <c r="AR10" s="6"/>
-      <c r="AS10" s="6"/>
-      <c r="AT10" s="6">
+      <c r="AQ10" s="5"/>
+      <c r="AR10" s="5"/>
+      <c r="AS10" s="5"/>
+      <c r="AT10" s="5">
         <v>11</v>
       </c>
-      <c r="AU10" s="6"/>
-      <c r="AV10" s="6"/>
-      <c r="AW10" s="6"/>
-      <c r="AX10" s="6">
+      <c r="AU10" s="5"/>
+      <c r="AV10" s="5"/>
+      <c r="AW10" s="5"/>
+      <c r="AX10" s="5">
         <v>12</v>
       </c>
-      <c r="AY10" s="6"/>
-      <c r="AZ10" s="6"/>
+      <c r="AY10" s="5"/>
+      <c r="AZ10" s="5"/>
     </row>
     <row r="11" spans="1:52" ht="148.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="6" t="s">
         <v>4</v>
       </c>
       <c r="C11" s="3">
@@ -928,7 +1013,7 @@
         <v>0.34375</v>
       </c>
       <c r="N11" s="3">
-        <f t="shared" si="0"/>
+        <f>(N9/4)/$B$3</f>
         <v>0.375</v>
       </c>
       <c r="O11" s="3">
@@ -1007,7 +1092,7 @@
         <f t="shared" si="0"/>
         <v>0.96875</v>
       </c>
-      <c r="AH11" s="4">
+      <c r="AH11" s="3">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1088,154 +1173,154 @@
       <c r="B12" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="F12" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="H12" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="I12" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="J12" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="K12" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="L12" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="M12" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="N12" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="O12" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="P12" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q12" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="R12" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="S12" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="T12" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="U12" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="V12" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="W12" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="X12" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="Y12" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="Z12" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="AA12" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="AB12" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="AC12" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="AD12" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="AE12" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="AF12" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="AG12" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="AH12" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="AI12" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="AJ12" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="AK12" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="AL12" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="AM12" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="AN12" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="AO12" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="AP12" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="AQ12" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="AR12" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="AS12" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="AT12" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="AU12" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="AV12" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="AW12" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="AX12" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="AY12" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="AZ12" s="22" t="s">
+      <c r="C12" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="J12" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="K12" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="L12" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="M12" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="N12" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="O12" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="P12" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q12" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="R12" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="S12" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="T12" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="U12" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="V12" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="W12" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="X12" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y12" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z12" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA12" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="AB12" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC12" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="AD12" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE12" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="AF12" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="AG12" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="AH12" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI12" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="AJ12" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="AK12" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="AL12" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="AM12" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="AN12" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="AO12" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="AP12" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="AQ12" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="AR12" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="AS12" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="AT12" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU12" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="AV12" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="AW12" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="AX12" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="AY12" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="AZ12" s="21" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1244,9 +1329,254 @@
         <v>5</v>
       </c>
     </row>
+    <row r="19" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="D19" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>0.125</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" s="5">
+        <f>COUNTA($B$20:B20)</f>
+        <v>1</v>
+      </c>
+      <c r="E20" s="5">
+        <f>D20-1</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="5">
+        <f>COUNTA($B$20:B21)</f>
+        <v>2</v>
+      </c>
+      <c r="E21" s="5">
+        <f t="shared" ref="E21:E34" si="1">D21-1</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>0.375</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" s="5">
+        <f>COUNTA($B$20:B22)</f>
+        <v>3</v>
+      </c>
+      <c r="E22" s="5">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" s="5">
+        <f>COUNTA($B$20:B23)</f>
+        <v>4</v>
+      </c>
+      <c r="E23" s="5">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24" s="5">
+        <f>COUNTA($B$20:B24)</f>
+        <v>5</v>
+      </c>
+      <c r="E24" s="5">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" s="5">
+        <f>COUNTA($B$20:B25)</f>
+        <v>6</v>
+      </c>
+      <c r="E25" s="5">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>0.875</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26" s="5">
+        <f>COUNTA($B$20:B26)</f>
+        <v>7</v>
+      </c>
+      <c r="E26" s="5">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>0.96875</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D27" s="5">
+        <f>COUNTA($B$20:B27)</f>
+        <v>8</v>
+      </c>
+      <c r="E27" s="5">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>1</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D28" s="5">
+        <f>COUNTA($B$20:B28)</f>
+        <v>9</v>
+      </c>
+      <c r="E28" s="5">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <v>1.0625</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D29" s="5">
+        <f>COUNTA($B$20:B29)</f>
+        <v>10</v>
+      </c>
+      <c r="E29" s="5">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
+        <v>1.15625</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D30" s="5">
+        <f>COUNTA($B$20:B30)</f>
+        <v>11</v>
+      </c>
+      <c r="E30" s="5">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <v>1.25</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D31" s="5">
+        <f>COUNTA($B$20:B31)</f>
+        <v>12</v>
+      </c>
+      <c r="E31" s="5">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>1.375</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D32" s="5">
+        <f>COUNTA($B$20:B32)</f>
+        <v>13</v>
+      </c>
+      <c r="E32" s="5">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D33" s="5">
+        <f>COUNTA($B$20:B33)</f>
+        <v>14</v>
+      </c>
+      <c r="E33" s="5">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B34" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D34" s="5">
+        <f>COUNTA($B$20:B34)</f>
+        <v>15</v>
+      </c>
+      <c r="E34" s="5">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="C11:AZ11">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>C$11=1</formula>
     </cfRule>
     <cfRule type="colorScale" priority="2">
@@ -1261,5 +1591,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>